<commit_message>
correction scrappe Ag LBMA
</commit_message>
<xml_diff>
--- a/metals_prices.xlsx
+++ b/metals_prices.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,6 +512,116 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>20900,00</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>20900,00</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>20900,00</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>20900,00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>20900,00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -528,7 +638,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -597,6 +707,116 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>24550,00</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>24550,00</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>24550,00</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>24550,00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>24550,00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -613,7 +833,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -682,6 +902,28 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>23,415</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>OZ</t>
         </is>
@@ -698,7 +940,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -767,6 +1009,28 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1969,65</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>OZ</t>
         </is>
@@ -1015,7 +1279,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1969.65</t>
+          <t>23,415</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1062,7 +1326,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1122,6 +1386,106 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1234</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1234</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1234</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1234</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1234</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -1138,7 +1502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1207,6 +1571,116 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>687,70</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>687,70</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>687,70</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>687,70</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>687,70</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -1223,7 +1697,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1283,6 +1757,106 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>123</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>123</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>123</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>123</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>123</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -1299,7 +1873,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1368,6 +1942,116 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>718,00</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>718,00</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>718,00</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>718,00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>718,00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -1384,7 +2068,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1453,6 +2137,116 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2234,00</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2234,00</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2234,00</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2234,00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2234,00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -1469,7 +2263,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1538,6 +2332,116 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>7910,00</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>7910,00</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>7910,00</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>7910,00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>7910,00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -1554,7 +2458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1623,6 +2527,116 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>873,13</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>873,13</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>873,13</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>873,13</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>873,13</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -1639,7 +2653,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1713,6 +2727,116 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9,27</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>9,27</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>9,27</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>9,27</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>25/05/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>9,27</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout de la fonction lancement auto
</commit_message>
<xml_diff>
--- a/metals_prices.xlsx
+++ b/metals_prices.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -671,6 +671,72 @@
         </is>
       </c>
       <c r="D11" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>20225,00</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>20225,00</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>20225,00</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -687,7 +753,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -910,6 +976,72 @@
         </is>
       </c>
       <c r="D11" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>25000,00</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>25000,00</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>25000,00</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -926,7 +1058,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1061,6 +1193,72 @@
         </is>
       </c>
       <c r="D7" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>24,535</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>24,535</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>24,535</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>OZ</t>
         </is>
@@ -1077,7 +1275,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1212,6 +1410,72 @@
         </is>
       </c>
       <c r="D7" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1942,3</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1942,3</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1942,3</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>OZ</t>
         </is>
@@ -1228,7 +1492,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1363,6 +1627,72 @@
         </is>
       </c>
       <c r="D7" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1067,00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1067,00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1067,00</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -1379,7 +1709,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1514,6 +1844,72 @@
         </is>
       </c>
       <c r="D7" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>783,00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>783,00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>783,00</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -1530,7 +1926,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1665,6 +2061,72 @@
         </is>
       </c>
       <c r="D7" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2412,50</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2412,50</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2412,50</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -1681,7 +2143,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1816,6 +2278,72 @@
         </is>
       </c>
       <c r="D7" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>27,20</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>27,20</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>27,20</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -2301,7 +2829,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2524,6 +3052,72 @@
         </is>
       </c>
       <c r="D11" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">725,64 </t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">725,64 </t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">725,64 </t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -2540,7 +3134,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2763,6 +3357,72 @@
         </is>
       </c>
       <c r="D11" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>714,80</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>714,80</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>714,80</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -2779,7 +3439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3002,6 +3662,72 @@
         </is>
       </c>
       <c r="D11" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>57 494,45</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>57 494,45</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>57 494,45</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -3018,7 +3744,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3241,6 +3967,72 @@
         </is>
       </c>
       <c r="D11" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>745,00</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>745,00</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>745,00</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -3257,7 +4049,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3480,6 +4272,72 @@
         </is>
       </c>
       <c r="D11" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2165,50</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2165,50</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2165,50</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -3496,7 +4354,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3719,6 +4577,72 @@
         </is>
       </c>
       <c r="D11" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>8359,50</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>8359,50</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>8359,50</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -3735,7 +4659,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -3958,6 +4882,72 @@
         </is>
       </c>
       <c r="D11" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>909,84</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>909,84</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>909,84</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -3974,7 +4964,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4202,6 +5192,72 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>9,35</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>9,35</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>9,35</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
btn disabled for saturday and sunday
</commit_message>
<xml_diff>
--- a/metals_prices.xlsx
+++ b/metals_prices.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="7" activeTab="16" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -26,7 +25,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RPA" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -66,7 +65,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -435,7 +434,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -447,13 +446,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -890,6 +889,248 @@
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>929,58</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>929,58</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>929,58</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>929,58</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>929,58</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>929,58</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>929,58</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>929,58</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -906,13 +1147,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1349,6 +1590,270 @@
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Semaine 37</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>9,45</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Semaine 37</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>9,45</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Semaine 37</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>9,45</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Semaine 37</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>9,45</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Semaine 37</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>9,45</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Semaine 37</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Semaine 37</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Semaine 37</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>9,45</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Semaine 37</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Semaine 37</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>9,45</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Semaine 37</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>9,45</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Semaine 37</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>9,45</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -1365,13 +1870,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <cols>
+    <col width="16.81640625" bestFit="1" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1793,6 +2301,270 @@
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Invalid date format</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>803,00</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Invalid date format</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>803,00</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Invalid date format</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>803,00</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Invalid date format</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>803,00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Invalid date format</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>803,00</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Invalid date format</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Invalid date format</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Invalid date format</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>803,00</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Invalid date format</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Invalid date format</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>803,00</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Invalid date format</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>803,00</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Invalid date format</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>803,00</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -1809,13 +2581,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2252,6 +3024,248 @@
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>765,00</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>765,00</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>765,00</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>765,00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>765,00</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>765,00</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>765,00</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>15/09/2023</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>765,00</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -2268,13 +3282,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2711,6 +3725,270 @@
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>20255,00</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>20255,00</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>20255,00</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>20255,00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>20255,00</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>20255,00</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>20255,00</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>20255,00</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>20255,00</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -2727,13 +4005,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -3170,6 +4448,270 @@
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>25650,00</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>25650,00</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>25650,00</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>25650,00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>25650,00</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>25650,00</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>25650,00</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>25650,00</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>25650,00</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -3186,13 +4728,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -3629,6 +5171,248 @@
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2551,00</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2551,00</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2551,00</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2551,00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2551,00</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2551,00</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2551,00</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2551,00</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -3647,11 +5431,11 @@
   </sheetPr>
   <dimension ref="A2:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -3666,7 +5450,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>27,48</t>
+          <t>Jour non valeur</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -3693,7 +5477,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">678,06 </t>
+          <t xml:space="preserve">695,74 </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -3720,7 +5504,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>22,905</t>
+          <t>22,64</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -3747,7 +5531,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2156,50</t>
+          <t>2192,50</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -3774,7 +5558,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1913,8</t>
+          <t>1901,75</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -3801,7 +5585,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>57 131,79</t>
+          <t>57 832,04</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3828,7 +5612,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1080,00</t>
+          <t>Jour non valeur</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -3855,7 +5639,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>8353,00</t>
+          <t>8423,00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -3882,7 +5666,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>920,04</t>
+          <t>Jour non valeur</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -3909,7 +5693,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>9,45</t>
+          <t>Jour non valeur</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -3936,7 +5720,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>801,00</t>
+          <t>Jour non valeur</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -3963,7 +5747,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>755,00</t>
+          <t>Jour non valeur</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3990,7 +5774,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>19485,00</t>
+          <t>20255,00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -4017,7 +5801,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>25200,00</t>
+          <t>25650,00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -4044,7 +5828,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2453,50</t>
+          <t>2551,00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -4069,13 +5853,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -4497,6 +6281,248 @@
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Semaine 37</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>27,48</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Semaine 37</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>27,48</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Semaine 37</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>27,48</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Semaine 37</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>27,48</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Semaine 37</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>27,48</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Semaine 37</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Semaine 37</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Semaine 37</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>27,48</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Semaine 37</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Semaine 37</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>27,48</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Semaine 37</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>27,48</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -4513,13 +6539,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -4956,6 +6982,270 @@
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">695,74 </t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">695,74 </t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">695,74 </t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">695,74 </t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">695,74 </t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">695,74 </t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">695,74 </t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">695,74 </t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">695,74 </t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -4972,13 +7262,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -5415,6 +7705,270 @@
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>22,64</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>22,64</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>22,64</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>22,64</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>22,64</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>22,64</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>22,64</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>22,64</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>22,64</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
         <is>
           <t>OZ</t>
         </is>
@@ -5431,13 +7985,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -5874,6 +8428,248 @@
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2192,50</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2192,50</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2192,50</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2192,50</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2192,50</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2192,50</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2192,50</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2192,50</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -5890,13 +8686,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -6333,6 +9129,270 @@
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>1901,75</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>1901,75</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>1901,75</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>1901,75</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>1901,75</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>1901,75</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>1901,75</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>1901,75</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>1901,75</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
         <is>
           <t>OZ</t>
         </is>
@@ -6349,13 +9409,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -6792,6 +9852,270 @@
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>57 832,04</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>57 832,04</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>57 832,04</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>57 832,04</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>57 832,04</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>57 832,04</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>57 832,04</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>57 832,04</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2023</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>57 832,04</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -6808,13 +10132,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -7251,6 +10575,248 @@
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>1093,00</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>1093,00</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>1093,00</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>1093,00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>1093,00</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>1093,00</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>1093,00</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>1093,00</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -7267,13 +10833,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -7710,6 +11276,248 @@
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>8423,00</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>8423,00</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>8423,00</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>8423,00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>8423,00</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>8423,00</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jour non valeur</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>8423,00</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>14/09/2023</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>8423,00</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
         <is>
           <t>TO</t>
         </is>

</xml_diff>

<commit_message>
ajout plage date + choix fonctions qui scrappent
</commit_message>
<xml_diff>
--- a/metals_prices.xlsx
+++ b/metals_prices.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="3" activeTab="11" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -25,7 +26,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RPA" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -65,7 +66,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -434,7 +435,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -446,23 +447,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D8"/>
+  <dimension ref="A2:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>923,18</t>
+          <t>891,95</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -479,12 +480,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>923,18</t>
+          <t>891,95</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -501,12 +502,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>923,18</t>
+          <t>891,95</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -523,12 +524,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>923,18</t>
+          <t>891,95</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -545,12 +546,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>923,18</t>
+          <t>891,95</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -567,12 +568,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>923,18</t>
+          <t>891,95</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -581,28 +582,6 @@
         </is>
       </c>
       <c r="D7" t="inlineStr">
-        <is>
-          <t>100KG</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>18/09/2023</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>923,18</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>€</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -619,23 +598,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Semaine 38</t>
+          <t xml:space="preserve"> Semaine 41</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>9,45</t>
+          <t>9,49</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -652,12 +631,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Semaine 38</t>
+          <t xml:space="preserve"> Semaine 41</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>9,45</t>
+          <t>9,49</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -674,12 +653,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Semaine 38</t>
+          <t xml:space="preserve"> Semaine 41</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>9,45</t>
+          <t>9,49</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -696,12 +675,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Semaine 38</t>
+          <t xml:space="preserve"> Semaine 41</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>9,45</t>
+          <t>9,49</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -718,12 +697,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Semaine 38</t>
+          <t xml:space="preserve"> Semaine 41</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9,45</t>
+          <t>9,49</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -732,28 +711,6 @@
         </is>
       </c>
       <c r="D6" t="inlineStr">
-        <is>
-          <t>KG</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Semaine 38</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>9,45</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>€</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -770,26 +727,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelCol="0"/>
-  <cols>
-    <col width="16.81640625" bestFit="1" customWidth="1" min="1" max="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Invalid date format</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>797,00</t>
+          <t>823,00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -806,12 +760,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Invalid date format</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>797,00</t>
+          <t>823,00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -828,12 +782,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Invalid date format</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>797,00</t>
+          <t>823,00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -850,12 +804,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Invalid date format</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>797,00</t>
+          <t>823,00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -872,12 +826,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Invalid date format</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>797,00</t>
+          <t>823,00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -886,28 +840,6 @@
         </is>
       </c>
       <c r="D6" t="inlineStr">
-        <is>
-          <t>100KG</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>18/09/2023</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>797,00</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>€</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -924,23 +856,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>759,00</t>
+          <t>738,00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -957,12 +889,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>759,00</t>
+          <t>738,00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -979,12 +911,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>759,00</t>
+          <t>738,00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1001,12 +933,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>759,00</t>
+          <t>738,00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1023,12 +955,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>759,00</t>
+          <t>738,00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1037,28 +969,6 @@
         </is>
       </c>
       <c r="D6" t="inlineStr">
-        <is>
-          <t>100KG</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>18/09/2023</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>759,00</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>€</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -1075,23 +985,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>18335,00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1108,12 +1018,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>18335,00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1130,12 +1040,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>18335,00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1152,12 +1062,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>18335,00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1174,12 +1084,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>18335,00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1188,28 +1098,6 @@
         </is>
       </c>
       <c r="D6" t="inlineStr">
-        <is>
-          <t>TO</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>18/09/2023</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -1226,23 +1114,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>25025,00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1259,12 +1147,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>25025,00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1281,12 +1169,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>25025,00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1303,12 +1191,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>25025,00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1325,12 +1213,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>25025,00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1347,12 +1235,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>25025,00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1361,6 +1249,28 @@
         </is>
       </c>
       <c r="D7" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>13/10/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>25025,00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -1377,23 +1287,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>2424,00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1410,12 +1320,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>2424,00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1432,12 +1342,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>2424,00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1454,66 +1364,60 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>TO</t>
+          <t>2424,00</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>12/10/2023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>TO</t>
+          <t>2445,50</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>11/10/2023</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>TO</t>
+          <t>2440,50</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>10/10/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2437,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>09/10/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2474,50</t>
         </is>
       </c>
     </row>
@@ -1528,82 +1432,82 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E16"/>
+  <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>360</t>
+          <t>ZN</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2360</t>
+          <t>3ZN1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>26,83</t>
+          <t>2424,00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>€</t>
+          <t>$</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>KG</t>
+          <t>TO</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AG</t>
+          <t>ZN</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1AG1</t>
+          <t>3ZN1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>2445,50</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>€</t>
+          <t>$</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>KG</t>
+          <t>TO</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AG</t>
+          <t>ZN</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1AG2</t>
+          <t>3ZN1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>2440,50</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1613,24 +1517,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>OZ</t>
+          <t>TO</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>AL</t>
+          <t>ZN</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3AL1</t>
+          <t>3ZN1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>2437,00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1647,17 +1551,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>ZN</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1AU2</t>
+          <t>3ZN1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>2474,50</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1666,276 +1570,6 @@
         </is>
       </c>
       <c r="E6" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>AU</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1AU3</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>€</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>KG</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>B16</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2B16</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1087,00</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>€</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>100KG</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>CU</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>3CU1</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>TO</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>CU</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>3CU3</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>923,18</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>€</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>100KG</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>CUB</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2CUB</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>9,45</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>€</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>KG</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>M30</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2M30</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>797,00</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>€</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>100KG</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>M37</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2M37</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>759,00</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>€</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>100KG</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>NI</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>3NI1</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>TO</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>SN</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>3SN1</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>TO</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>ZN</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>3ZN1</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -1958,9 +1592,19 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Semaine 41</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>25,70</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>€</t>
@@ -1973,6 +1617,16 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Semaine 41</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>25,70</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>€</t>
@@ -1987,12 +1641,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Semaine 38</t>
+          <t>Semaine 41</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>26,83</t>
+          <t>25,70</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2009,12 +1663,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Semaine 38</t>
+          <t>Semaine 41</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>26,83</t>
+          <t>25,70</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2031,12 +1685,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Semaine 38</t>
+          <t>Semaine 41</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>26,83</t>
+          <t>25,70</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2053,12 +1707,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Semaine 38</t>
+          <t>Semaine 41</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>26,83</t>
+          <t>25,70</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2083,23 +1737,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D8"/>
+  <dimension ref="A2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 19/09/2023</t>
+          <t xml:space="preserve"> 13/10/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t xml:space="preserve">674,84 </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2116,12 +1770,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 19/09/2023</t>
+          <t xml:space="preserve"> 13/10/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t xml:space="preserve">674,84 </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2138,12 +1792,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 19/09/2023</t>
+          <t xml:space="preserve"> 13/10/2023</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t xml:space="preserve">674,84 </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2160,12 +1814,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 19/09/2023</t>
+          <t xml:space="preserve"> 13/10/2023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t xml:space="preserve">674,84 </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2182,12 +1836,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 19/09/2023</t>
+          <t xml:space="preserve"> 13/10/2023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t xml:space="preserve">674,84 </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2196,50 +1850,6 @@
         </is>
       </c>
       <c r="D6" t="inlineStr">
-        <is>
-          <t>KG</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 19/09/2023</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>€</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>KG</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 19/09/2023</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>€</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -2256,23 +1866,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D8"/>
+  <dimension ref="A2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>22,08</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2289,12 +1899,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>22,08</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2311,12 +1921,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13.10.2023</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>22,08</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2333,12 +1943,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>22,08</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2355,12 +1965,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>22,08</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2369,50 +1979,6 @@
         </is>
       </c>
       <c r="D6" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>18/09/2023</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>18/09/2023</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
         <is>
           <t>OZ</t>
         </is>
@@ -2435,17 +2001,17 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>2176,00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2462,12 +2028,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>2176,00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2484,12 +2050,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>2176,00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2506,12 +2072,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>2176,00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2528,12 +2094,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>2176,00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2550,12 +2116,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>2176,00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2572,12 +2138,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>2176,00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2602,23 +2168,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D8"/>
+  <dimension ref="A2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13.10.2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>1909,2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2635,12 +2201,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13.10.2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>1909,2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2657,12 +2223,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>1909,2</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2679,12 +2245,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>1909,2</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2701,12 +2267,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>1909,2</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2715,50 +2281,6 @@
         </is>
       </c>
       <c r="D6" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>18/09/2023</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>18/09/2023</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
         <is>
           <t>OZ</t>
         </is>
@@ -2781,17 +2303,17 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 19/09/2023</t>
+          <t xml:space="preserve"> 13/10/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>57 543,97</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2808,12 +2330,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 19/09/2023</t>
+          <t xml:space="preserve"> 13/10/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>57 543,97</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2830,12 +2352,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 19/09/2023</t>
+          <t xml:space="preserve"> 13/10/2023</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>57 543,97</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2852,12 +2374,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 19/09/2023</t>
+          <t xml:space="preserve"> 13/10/2023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>57 543,97</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2874,12 +2396,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 19/09/2023</t>
+          <t xml:space="preserve"> 13/10/2023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>57 543,97</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2896,12 +2418,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 19/09/2023</t>
+          <t xml:space="preserve"> 13/10/2023</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>57 543,97</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2918,12 +2440,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 19/09/2023</t>
+          <t xml:space="preserve"> 16/10/2023</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>58 411,71</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2948,23 +2470,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D8"/>
+  <dimension ref="A2:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1087,00</t>
+          <t>1056,00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2981,12 +2503,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1087,00</t>
+          <t>1056,00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -3003,12 +2525,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1087,00</t>
+          <t>1056,00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -3025,12 +2547,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1087,00</t>
+          <t>1056,00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3047,12 +2569,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1087,00</t>
+          <t>1056,00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -3069,12 +2591,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1087,00</t>
+          <t>1056,00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3091,12 +2613,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>E</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1087,00</t>
+          <t>1056,00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -3105,6 +2627,72 @@
         </is>
       </c>
       <c r="D8" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1056,00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1056,00</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1056,00</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -3121,23 +2709,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D8"/>
+  <dimension ref="A2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>7891,00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3154,12 +2742,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>7891,00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -3176,12 +2764,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>7891,00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -3198,12 +2786,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>7891,00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3220,12 +2808,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18/09/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jour non valeur</t>
+          <t>7891,00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -3234,50 +2822,6 @@
         </is>
       </c>
       <c r="D6" t="inlineStr">
-        <is>
-          <t>TO</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>18/09/2023</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>TO</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>18/09/2023</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Jour non valeur</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
         <is>
           <t>TO</t>
         </is>

</xml_diff>

<commit_message>
correctif scrapping functions 3SN1 3NI1
</commit_message>
<xml_diff>
--- a/metals_prices.xlsx
+++ b/metals_prices.xlsx
@@ -2401,7 +2401,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D116"/>
+  <dimension ref="A2:D119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
@@ -4934,6 +4934,57 @@
         </is>
       </c>
       <c r="D116" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>18/10/2023</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>18/10/2023</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>18/10/2023</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -6707,7 +6758,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D93"/>
+  <dimension ref="A2:D99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
@@ -8742,6 +8793,108 @@
         </is>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>18/10/2023</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>18.470,00</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>19/10/2023</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>18.285,00</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>19/10/2023</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>18.285,00</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -8753,7 +8906,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D97"/>
+  <dimension ref="A2:D103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
@@ -10868,6 +11021,138 @@
         </is>
       </c>
       <c r="D97" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>18/10/2023</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>25.450,00</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>18/10/2023</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>25.450,00</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>18/10/2023</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>25.450,00</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>18/10/2023</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>25.450,00</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>18/10/2023</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>25.450,00</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>19/10/2023</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>25.075,00</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -12949,7 +13234,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E4"/>
+  <dimension ref="A2:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
@@ -12970,7 +13255,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>18.470,00</t>
+          <t>18.285,00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -12997,7 +13282,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>25.450,00</t>
+          <t>25.075,00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -13006,33 +13291,6 @@
         </is>
       </c>
       <c r="E3" t="inlineStr">
-        <is>
-          <t>TO</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ZN</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>3ZN1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2431,00</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
         <is>
           <t>TO</t>
         </is>

</xml_diff>

<commit_message>
verification en main pour la version
</commit_message>
<xml_diff>
--- a/metals_prices.xlsx
+++ b/metals_prices.xlsx
@@ -6707,7 +6707,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D93"/>
+  <dimension ref="A2:D94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
@@ -8742,6 +8742,18 @@
         </is>
       </c>
     </row>
+    <row r="94">
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -8753,7 +8765,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D97"/>
+  <dimension ref="A2:D98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
@@ -10868,6 +10880,18 @@
         </is>
       </c>
       <c r="D97" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -10884,7 +10908,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D94"/>
+  <dimension ref="A2:D95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -12933,6 +12957,28 @@
         </is>
       </c>
       <c r="D94" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>23/10/2023</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>2404,00</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -12968,11 +13014,6 @@
           <t>3NI1</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>18.470,00</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>$</t>
@@ -12995,11 +13036,6 @@
           <t>3SN1</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>25.450,00</t>
-        </is>
-      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>$</t>
@@ -13024,7 +13060,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2431,00</t>
+          <t>2404,00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">

</xml_diff>

<commit_message>
ajout des fonctions ZLME et EURX
</commit_message>
<xml_diff>
--- a/metals_prices.xlsx
+++ b/metals_prices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="16440" tabRatio="600" firstSheet="1" activeTab="16" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="3" activeTab="17" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -22,7 +22,9 @@
     <sheet name="3NI1" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="3SN1" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="3ZN1" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="RPA" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="ZLME" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="EURX" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="RPA" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -32,13 +34,26 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Abadi"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Abadi"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,7 +64,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -57,12 +72,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +482,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D84"/>
+  <dimension ref="A2:D87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
@@ -2275,6 +2311,72 @@
         </is>
       </c>
       <c r="D84" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>890,28</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>890,28</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>891,96</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -2291,7 +2393,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D13"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2566,6 +2668,28 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Semaine 46</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>9,45</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2577,7 +2701,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D120"/>
+  <dimension ref="A2:D123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
@@ -5193,6 +5317,72 @@
         </is>
       </c>
       <c r="D120" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>776,00</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>776,00</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>776,00</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -5209,7 +5399,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D85"/>
+  <dimension ref="A2:D88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
@@ -7060,6 +7250,72 @@
         </is>
       </c>
       <c r="D85" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>741,00</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>741,00</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>740,00</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -7076,7 +7332,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D100"/>
+  <dimension ref="A2:D103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
@@ -9255,6 +9511,72 @@
         </is>
       </c>
     </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>17170,00</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>17170,00</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>17000,00</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -9266,7 +9588,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D104"/>
+  <dimension ref="A2:D107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
@@ -11525,6 +11847,72 @@
         </is>
       </c>
       <c r="D104" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>24275,00</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>24275,00</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>24750,00</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -11541,7 +11929,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D103"/>
+  <dimension ref="A2:D106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -13788,6 +14176,72 @@
         </is>
       </c>
       <c r="D103" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>2584,00</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>2584,00</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>2538,00</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -13804,9 +14258,443 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E16"/>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Déb.Val</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Certain</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>de</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>06/11/2023</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1,07450</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>07/11/2023</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1,06790</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>08/11/2023</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1,06680</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>09/11/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1,06900</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1,06820</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1,06730</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1,06730</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1,06730</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Déb.Val</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Certain</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>de</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>06/11/2023</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1,07410</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>07/11/2023</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1,06860</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>08/11/2023</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1,06710</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>09/11/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1,06910</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1,06830</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1,06700</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1,06700</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1,06700</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -13825,7 +14713,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>24,64</t>
+          <t>24,43</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -13852,7 +14740,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">812,90 </t>
+          <t xml:space="preserve">797,08 </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -13879,7 +14767,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>22,495</t>
+          <t>22,075</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -13906,7 +14794,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2205,50</t>
+          <t>2220,50</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -13933,7 +14821,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1941,65</t>
+          <t>1931,15</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -13960,7 +14848,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>59 233,00</t>
+          <t>58 648,00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -13987,7 +14875,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1047,00</t>
+          <t>1051,00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -14014,7 +14902,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>8006,00</t>
+          <t>8014,50</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -14041,7 +14929,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>890,28</t>
+          <t>891,96</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -14068,7 +14956,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>9,47</t>
+          <t>9,45</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -14122,7 +15010,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>741,00</t>
+          <t>740,00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -14149,7 +15037,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>17170,00</t>
+          <t>17000,00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -14176,7 +15064,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>24275,00</t>
+          <t>24750,00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -14203,7 +15091,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2584,00</t>
+          <t>2538,00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -14214,6 +15102,60 @@
       <c r="E16" t="inlineStr">
         <is>
           <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ZLME</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ZLME</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>1,06730</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>EURX</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>EURX</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1,06700</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>EUR</t>
         </is>
       </c>
     </row>
@@ -14228,7 +15170,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D16"/>
+  <dimension ref="A2:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14561,6 +15503,50 @@
         </is>
       </c>
       <c r="D16" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Semaine 46</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>24,43</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Semaine 46</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>24,43</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -14577,7 +15563,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D86"/>
+  <dimension ref="A2:D90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
@@ -16306,6 +17292,94 @@
         </is>
       </c>
       <c r="D86" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">812,90 </t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">812,90 </t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">797,08 </t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">797,08 </t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -16322,7 +17396,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D84"/>
+  <dimension ref="A2:D88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
@@ -18011,6 +19085,94 @@
         </is>
       </c>
       <c r="D84" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>22,495</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>22,495</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>22,075</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>22,075</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
         <is>
           <t>OZ</t>
         </is>
@@ -18027,7 +19189,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D84"/>
+  <dimension ref="A2:D88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A52" sqref="A3:XFD52"/>
@@ -19856,6 +21018,94 @@
         </is>
       </c>
       <c r="D84" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>2205,50</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>2205,50</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>2220,50</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>2220,50</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -19872,7 +21122,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D84"/>
+  <dimension ref="A2:D88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
@@ -21561,6 +22811,94 @@
         </is>
       </c>
       <c r="D84" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>1941,65</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>1941,65</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>1931,15</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>1931,15</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
         <is>
           <t>OZ</t>
         </is>
@@ -21577,7 +22915,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D86"/>
+  <dimension ref="A2:D89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
@@ -23306,6 +24644,72 @@
         </is>
       </c>
       <c r="D86" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>59 233,00</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>59 233,00</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>58 648,00</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -23322,7 +24726,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D84"/>
+  <dimension ref="A2:D87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
@@ -25151,6 +26555,72 @@
         </is>
       </c>
       <c r="D84" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>1047,00</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>1047,00</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>1051,00</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -25167,7 +26637,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D110"/>
+  <dimension ref="A2:D113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
@@ -27573,6 +29043,72 @@
         </is>
       </c>
     </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>8006,00</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>8006,00</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>13/11/2023</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>8014,50</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Date en A1 et jour de la semaine en B1 pour RPA
</commit_message>
<xml_diff>
--- a/metals_prices.xlsx
+++ b/metals_prices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="3" activeTab="17" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-16310" windowWidth="29020" windowHeight="15700" tabRatio="600" firstSheet="3" activeTab="18" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -33,7 +33,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <name val="Calibri"/>
@@ -91,7 +93,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -99,6 +101,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,7 +485,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D87"/>
+  <dimension ref="A2:D93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
@@ -2377,6 +2380,138 @@
         </is>
       </c>
       <c r="D87" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>05/12/2023</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>904,41</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>922,31</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>922,31</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>922,31</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>922,31</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>922,31</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -2393,7 +2528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D14"/>
+  <dimension ref="A2:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2690,6 +2825,116 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Semaine 49</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>9,59</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Semaine 5</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>9,40</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Semaine 5</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>9,40</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Semaine 5</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>9,40</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Semaine 5</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>9,40</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2701,7 +2946,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D123"/>
+  <dimension ref="A2:D128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
@@ -5383,6 +5628,116 @@
         </is>
       </c>
       <c r="D123" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>05/12/2023</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>780,00</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>795,00</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>795,00</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>847,00</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>847,00</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -5399,7 +5754,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D88"/>
+  <dimension ref="A2:D93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
@@ -7316,6 +7671,116 @@
         </is>
       </c>
       <c r="D88" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>05/12/2023</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>742,00</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>756,00</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>756,00</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>756,00</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>756,00</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -7332,7 +7797,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D103"/>
+  <dimension ref="A2:D108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
@@ -9577,6 +10042,116 @@
         </is>
       </c>
     </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>05/12/2023</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>16060,00</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>15985,00</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>15985,00</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>15985,00</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>15985,00</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -9588,7 +10163,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D107"/>
+  <dimension ref="A2:D112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
@@ -11913,6 +12488,116 @@
         </is>
       </c>
       <c r="D107" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>05/12/2023</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>23750,00</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>25700,00</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>25700,00</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>25700,00</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>25700,00</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -11929,7 +12614,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D106"/>
+  <dimension ref="A2:D111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -14242,6 +14927,116 @@
         </is>
       </c>
       <c r="D106" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>05/12/2023</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>2421,00</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>2478,00</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>2478,00</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>2478,00</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>2478,00</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -14258,7 +15053,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -14459,6 +15254,116 @@
         </is>
       </c>
       <c r="D9" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>05/12/2023</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1,08140</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1,08150</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1,08150</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1,08150</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1,08150</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>EUR</t>
         </is>
@@ -14475,9 +15380,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -14676,6 +15581,116 @@
         </is>
       </c>
       <c r="D9" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>05/12/2023</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1,08170</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1,08140</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1,08140</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1,08140</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1,08140</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>EUR</t>
         </is>
@@ -14692,14 +15707,29 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <cols>
+    <col width="16.7265625" bestFit="1" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>jeudi</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
@@ -14713,7 +15743,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>24,43</t>
+          <t>21,39</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -14740,7 +15770,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">797,08 </t>
+          <t xml:space="preserve">809,04 </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -14767,7 +15797,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>22,075</t>
+          <t>22,67</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -14794,7 +15824,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2220,50</t>
+          <t>2212,50</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -14821,7 +15851,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1931,15</t>
+          <t>2045,85</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -14848,7 +15878,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>58 648,00</t>
+          <t>61 062,00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -14875,7 +15905,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1051,00</t>
+          <t>1084,00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -14902,7 +15932,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>8014,50</t>
+          <t>8437,00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -14929,7 +15959,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>891,96</t>
+          <t>922,31</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -14956,7 +15986,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>9,45</t>
+          <t>9,40</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -14983,7 +16013,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>776,00</t>
+          <t>847,00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -15010,7 +16040,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>740,00</t>
+          <t>756,00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -15037,7 +16067,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>17000,00</t>
+          <t>15985,00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -15064,7 +16094,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>24750,00</t>
+          <t>25700,00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -15091,7 +16121,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2538,00</t>
+          <t>2478,00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -15118,7 +16148,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1,06730</t>
+          <t>1,08150</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -15145,7 +16175,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1,06700</t>
+          <t>1,08140</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -15170,7 +16200,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D18"/>
+  <dimension ref="A2:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15547,6 +16577,226 @@
         </is>
       </c>
       <c r="D18" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Semaine 49</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>22,15</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Semaine 5</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>21,39</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Semaine 5</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>21,39</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Semaine 5</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>21,39</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Semaine 5</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>21,39</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Semaine 5</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>21,39</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Semaine 5</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>21,39</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Semaine 5</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>21,39</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Semaine 5</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>21,39</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Semaine 5</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>21,39</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -15563,7 +16813,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D90"/>
+  <dimension ref="A2:D98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
@@ -17380,6 +18630,182 @@
         </is>
       </c>
       <c r="D90" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>05/12/2023</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">865,37 </t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">809,04 </t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">809,04 </t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">809,04 </t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">809,04 </t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t xml:space="preserve">809,04 </t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">809,04 </t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t xml:space="preserve">809,04 </t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -17396,7 +18822,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D88"/>
+  <dimension ref="A2:D96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
@@ -19173,6 +20599,182 @@
         </is>
       </c>
       <c r="D88" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>05/12/2023</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>24,27</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>22,67</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>22,67</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>22,67</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>22,67</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>22,67</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>22,67</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>22,67</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
         <is>
           <t>OZ</t>
         </is>
@@ -19189,7 +20791,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D88"/>
+  <dimension ref="A2:D94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A52" sqref="A3:XFD52"/>
@@ -21106,6 +22708,138 @@
         </is>
       </c>
       <c r="D88" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>05/12/2023</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>2121,50</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>2212,50</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>2212,50</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>2212,50</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>2212,50</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>2212,50</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -21122,7 +22856,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D88"/>
+  <dimension ref="A2:D94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
@@ -22899,6 +24633,138 @@
         </is>
       </c>
       <c r="D88" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>05/12/2023</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>2023,35</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>2045,85</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>2045,85</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>2045,85</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>2045,85</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>2045,85</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
         <is>
           <t>OZ</t>
         </is>
@@ -22915,7 +24781,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D89"/>
+  <dimension ref="A2:D95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
@@ -24710,6 +26576,138 @@
         </is>
       </c>
       <c r="D89" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>05/12/2023</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>60 417,00</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>61 062,00</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>61 062,00</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>61 062,00</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>61 062,00</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>61 062,00</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -24726,7 +26724,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D87"/>
+  <dimension ref="A2:D93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
@@ -26621,6 +28619,138 @@
         </is>
       </c>
       <c r="D87" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>05/12/2023</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>1055,00</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>1084,00</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>1084,00</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>1084,00</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>1084,00</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>1084,00</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -26637,7 +28767,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D113"/>
+  <dimension ref="A2:D119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
@@ -29109,6 +31239,138 @@
         </is>
       </c>
     </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>05/12/2023</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>8259,00</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>8437,00</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>8437,00</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>8437,00</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>8437,00</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>8437,00</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add new function CUSN6
</commit_message>
<xml_diff>
--- a/metals_prices.xlsx
+++ b/metals_prices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-16310" windowWidth="29020" windowHeight="15700" tabRatio="600" firstSheet="3" activeTab="18" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17280" tabRatio="600" firstSheet="3" activeTab="19" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="ZLME" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="EURX" sheetId="18" state="visible" r:id="rId18"/>
     <sheet name="RPA" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="CUSN" sheetId="20" state="visible" r:id="rId20"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -473,7 +474,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -485,13 +486,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D93"/>
+  <dimension ref="A2:D95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2512,6 +2513,50 @@
         </is>
       </c>
       <c r="D93" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>1032,41</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>1032,41</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -2528,13 +2573,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D19"/>
+  <dimension ref="A2:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="11" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -2930,6 +2975,50 @@
         </is>
       </c>
       <c r="D19" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Semaine 15</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>10,07</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Semaine 15</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>10,07</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -2946,13 +3035,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D128"/>
+  <dimension ref="A2:D130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -5738,6 +5827,50 @@
         </is>
       </c>
       <c r="D128" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>869,00</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>869,00</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -5754,13 +5887,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D93"/>
+  <dimension ref="A2:D95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -7781,6 +7914,50 @@
         </is>
       </c>
       <c r="D93" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>844,00</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>844,00</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -7797,15 +7974,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D108"/>
+  <dimension ref="A2:D110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="13.90625" customWidth="1" min="1" max="1"/>
+    <col width="13.83203125" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -10147,6 +10324,50 @@
         </is>
       </c>
       <c r="D108" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>17780,00</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>17780,00</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -10163,13 +10384,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D112"/>
+  <dimension ref="A2:D114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -12598,6 +12819,50 @@
         </is>
       </c>
       <c r="D112" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>32975,00</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>32975,00</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -12614,13 +12879,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D111"/>
+  <dimension ref="A2:D113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -15037,6 +15302,50 @@
         </is>
       </c>
       <c r="D111" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>2848,00</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>2848,00</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -15053,13 +15362,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
@@ -15364,6 +15673,50 @@
         </is>
       </c>
       <c r="D14" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1,06510</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1,06510</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
         <is>
           <t>EUR</t>
         </is>
@@ -15380,13 +15733,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
@@ -15691,6 +16044,50 @@
         </is>
       </c>
       <c r="D14" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1,06520</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1,06520</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
         <is>
           <t>EUR</t>
         </is>
@@ -15707,26 +16104,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="16.7265625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="16.6640625" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>01/02/2024</t>
+          <t>12/04/2024</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>jeudi</t>
+          <t>Vendredi</t>
         </is>
       </c>
     </row>
@@ -15743,7 +16140,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>21,39</t>
+          <t>22,59</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -15770,7 +16167,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">809,04 </t>
+          <t xml:space="preserve">1 051,71 </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -15797,7 +16194,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>22,67</t>
+          <t>29,025</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -15824,7 +16221,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2212,50</t>
+          <t>2443,00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -15851,7 +16248,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2045,85</t>
+          <t>2401,5</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -15878,7 +16275,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>61 062,00</t>
+          <t>72 665,00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -15905,7 +16302,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1084,00</t>
+          <t>1238,00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -15932,7 +16329,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>8437,00</t>
+          <t>9402,00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -15959,7 +16356,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>922,31</t>
+          <t>1032,41</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -15986,7 +16383,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>9,40</t>
+          <t>10,07</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -16013,7 +16410,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>847,00</t>
+          <t>869,00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -16040,7 +16437,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>756,00</t>
+          <t>844,00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -16067,7 +16464,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>15985,00</t>
+          <t>17780,00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -16094,7 +16491,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>25700,00</t>
+          <t>32975,00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -16121,7 +16518,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2478,00</t>
+          <t>2848,00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -16148,7 +16545,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1,08150</t>
+          <t>1,06510</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -16175,7 +16572,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1,08140</t>
+          <t>1,06520</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -16186,6 +16583,33 @@
       <c r="E18" t="inlineStr">
         <is>
           <t>EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>CUSN</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>CUSN</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>11681,41</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>TO</t>
         </is>
       </c>
     </row>
@@ -16200,13 +16624,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D28"/>
+  <dimension ref="A2:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -16802,8 +17226,154 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Semaine 15</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>22,59</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Semaine 15</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>22,59</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R33" sqref="R33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Semaine 15</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Valeur non trouvée</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>11681,41</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11681,41</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -16813,13 +17383,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D98"/>
+  <dimension ref="A2:D100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -18806,6 +19376,50 @@
         </is>
       </c>
       <c r="D98" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 051,71 </t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 051,71 </t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -18822,13 +19436,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D96"/>
+  <dimension ref="A2:D98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -20775,6 +21389,50 @@
         </is>
       </c>
       <c r="D96" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>29,025</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>29,025</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
         <is>
           <t>OZ</t>
         </is>
@@ -20791,13 +21449,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D94"/>
+  <dimension ref="A2:D96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A52" sqref="A3:XFD52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -22840,6 +23498,50 @@
         </is>
       </c>
       <c r="D94" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>2443,00</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>2443,00</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
         <is>
           <t>TO</t>
         </is>
@@ -22856,13 +23558,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D94"/>
+  <dimension ref="A2:D96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -24765,6 +25467,50 @@
         </is>
       </c>
       <c r="D94" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>2401,5</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>OZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>2401,5</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
         <is>
           <t>OZ</t>
         </is>
@@ -24781,13 +25527,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D95"/>
+  <dimension ref="A2:D97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -26708,6 +27454,50 @@
         </is>
       </c>
       <c r="D95" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>72 665,00</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>72 665,00</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
         <is>
           <t>KG</t>
         </is>
@@ -26724,13 +27514,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D93"/>
+  <dimension ref="A2:D95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -28751,6 +29541,50 @@
         </is>
       </c>
       <c r="D93" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>1238,00</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>100KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>1238,00</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>€</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
         <is>
           <t>100KG</t>
         </is>
@@ -28767,13 +29601,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D119"/>
+  <dimension ref="A2:D121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -31366,6 +32200,50 @@
         </is>
       </c>
       <c r="D119" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>9402,00</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>12/04/2024</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>9402,00</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
         <is>
           <t>TO</t>
         </is>

</xml_diff>